<commit_message>
Add to-do list via upload
</commit_message>
<xml_diff>
--- a/Documents/1045-Group1– To-do list for Homework Number 4 & 5.xlsx
+++ b/Documents/1045-Group1– To-do list for Homework Number 4 & 5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seeram\Desktop\School shit\CSCI 331\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ridh\Desktop\QC Classes\Fall 2025\CSCI 331 - Database Systems\Homework 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2011380-8225-41A9-A59A-1026E1179F1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E193E9-39F3-45EB-9C7F-2300CBA5ED63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Giorgos Stefanis" sheetId="1" r:id="rId1"/>
@@ -1642,7 +1642,7 @@
   <dimension ref="B1:H16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B6" sqref="B6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1973,7 +1973,7 @@
   <dimension ref="B1:H16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2965,7 +2965,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -2977,7 +2977,7 @@
     <col min="5" max="5" width="16.28515625" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.4">
@@ -3020,10 +3020,10 @@
       <c r="G4" s="15"/>
       <c r="H4" s="16"/>
     </row>
-    <row r="6" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="17" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -3078,7 +3078,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="8">
         <v>1</v>
@@ -3122,7 +3122,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="8">
         <v>1</v>
@@ -3144,7 +3144,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="47.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="8">
         <v>1</v>
@@ -3166,7 +3166,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="8">
         <v>1</v>
@@ -3188,7 +3188,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="8">
         <v>1</v>
@@ -3210,7 +3210,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="47.25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="8">
         <v>1</v>
@@ -3232,7 +3232,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="47.25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="8">
         <v>1</v>
@@ -3277,7 +3277,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter To be completed by person Name in this cell" sqref="F3:H3" xr:uid="{4CBA3FED-50EE-46A2-9666-9D4E524A6986}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter deadline Date in cell at right" sqref="B4:E4" xr:uid="{35C96656-9501-4204-BE40-9E90DDBF6E17}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter deadline Date in this cell" sqref="F4:H4" xr:uid="{A802B69D-98A7-4589-833F-822C46CD99E9}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter details of Project 1 in table below" sqref="B6:H6" xr:uid="{374326C9-DFCB-4148-B9F9-A58F4A97DD15}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter details of Project 1 in table below" sqref="B6:H6" xr:uid="{0C2F7F68-6F6B-4688-9327-2FF06E4E7352}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Percent done in this column under this heading. Data bar showing Percent done is automatically updated in each row. Use heading filters to find specific entries" sqref="B7" xr:uid="{972A0694-5162-4C74-B414-967AF21155FC}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter project Phase in this column under this heading" sqref="C7" xr:uid="{61F400D3-9DAC-44E1-AFEF-4532D3A466C1}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Due By date in this column under this heading" sqref="D7:G7" xr:uid="{0651D88E-2421-49C0-9AA0-91EE411175D4}"/>

</xml_diff>